<commit_message>
finish updating acc tests
</commit_message>
<xml_diff>
--- a/doc/ver1_fixes/AcceptanceTests - New.xlsx
+++ b/doc/ver1_fixes/AcceptanceTests - New.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$98</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="290">
   <si>
     <t>use case</t>
   </si>
@@ -258,12 +258,6 @@
   </si>
   <si>
     <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #watchCart</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_watchCart1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_watchCart2()</t>
   </si>
   <si>
     <t xml:space="preserve">עגלת המשתמש מכילה את המוצרים id_1, id_2 בלבד. המשתמש בוחר לערוך את העגלה ולהוסיף עוד 2- פריטים מהמוצר id_1 </t>
@@ -571,9 +565,6 @@
     <t>המערכת מחזירה הודעה על זה שניתן להסיר רק בעלי חנויות</t>
   </si>
   <si>
-    <t>מנוי id_1 לא מוגדר כבעל החנות וכל מי שהוא מינה אינם העלי החנות גם כן</t>
-  </si>
-  <si>
     <t>משתמש מזוהה כבעל חנות והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי, מבקשים הרשאה לערוך מוצרים. יש ממנה יחיד לחנות</t>
   </si>
   <si>
@@ -700,9 +691,6 @@
     <t>המערכת מחזירה הודעת שגיאה על כך שהמשתמש שאותו רוצים להסיר לא קיים במערכת</t>
   </si>
   <si>
-    <t>משתמש אשר אינו מזוהה כמנהל מערכת מנסה להסיר משתמש אשר לא קיים במערכת id_1</t>
-  </si>
-  <si>
     <t>המערכת מחזירה הודעת שגיאה על כך שרק מנהל המערכת מורשה למחוק משתמשים</t>
   </si>
   <si>
@@ -772,18 +760,12 @@
     <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אך תיאור החנות קצר מדי</t>
   </si>
   <si>
-    <t>המערכת מודיעה כי תיאור חנות צריך לכלול לפחות 150 תווים. לא נפתחת חנות id_1</t>
-  </si>
-  <si>
     <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שמחירו שלילי.</t>
   </si>
   <si>
     <t>המערכת מחווה כי מחיר מוצר חייב להיות חיובי. המוצר לא נוסף לחנות.</t>
   </si>
   <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שכמותו שלילית.</t>
-  </si>
-  <si>
     <t>המערכת מחווה כי כמות מוצר חייבת להיות חיובית. המוצר לא נוסף לחנות.</t>
   </si>
   <si>
@@ -812,13 +794,124 @@
   </si>
   <si>
     <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_setup5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_login4()</t>
+  </si>
+  <si>
+    <t>חיפוש לפי שם מוצר ריק</t>
+  </si>
+  <si>
+    <t>המערכת תציג את כל המוצרים במערכת</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_searchItem7()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_searchItem8()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_searchItem9()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_watchCart()   test_removeItemFromCart</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemQuantityInCart()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemQuantityInCart2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_logout3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore5()</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אך החוקים יוצרים סתירה</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי החוקים יוצרים סתירה. לא נפתחת חנות id_1</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי תיאור חנות צריך לכלול לפחות 20 תווים. לא נפתחת חנות id_1</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore6()</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שכמותו שלילית</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שכמותו אינה שלמה</t>
+  </si>
+  <si>
+    <t>המערכת מחווה כי כמות מוצר חייבת להיות שלמה. המוצר לא נוסף לחנות.</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore6()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager4()</t>
+  </si>
+  <si>
+    <t>מנוי id_1 לא מוגדר כבעל החנות וכל מי שהוא מינה אינם בעלי החנות גם כן</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeManager3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeItemFromStore4()</t>
+  </si>
+  <si>
+    <t>משתמש אשר מזוהה כמנהל מערכת מנסה להסיר משתמש אשר לא קיים במערכת id_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -834,8 +927,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFFFC66D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -992,6 +1091,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1042,7 +1147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1151,6 +1256,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1481,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F275"/>
+  <dimension ref="A1:F278"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1494,7 +1605,7 @@
     <col min="3" max="3" width="42.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="53.25" style="2" customWidth="1"/>
     <col min="5" max="5" width="57" style="2" customWidth="1"/>
-    <col min="6" max="6" width="48.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="57.875" style="2" customWidth="1"/>
     <col min="7" max="16384" width="8.75" style="2"/>
   </cols>
   <sheetData>
@@ -1575,7 +1686,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1595,7 +1706,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1615,7 +1726,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1738,7 +1849,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <v>2.2999999999999998</v>
       </c>
@@ -1753,6 +1864,9 @@
       </c>
       <c r="E13" s="12" t="s">
         <v>29</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -1783,148 +1897,156 @@
         <v>2</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>64</v>
+        <v>254</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="7"/>
+        <v>255</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="17">
+      <c r="A16" s="16">
         <v>2.5</v>
       </c>
       <c r="B16" s="2">
         <v>3</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>37</v>
+      <c r="C16" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>47</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="17">
         <v>2.5</v>
       </c>
       <c r="B17" s="2">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="17">
+      <c r="A18" s="16">
         <v>2.5</v>
       </c>
       <c r="B18" s="2">
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>47</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="16">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="17">
         <v>2.5</v>
       </c>
       <c r="B19" s="2">
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>47</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="17">
+      <c r="A20" s="16">
         <v>2.5</v>
       </c>
       <c r="B20" s="2">
         <v>7</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>41</v>
+      <c r="C20" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>47</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>53</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="16">
+      <c r="A21" s="17">
         <v>2.5</v>
       </c>
       <c r="B21" s="2">
         <v>8</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="16">
+        <v>2.5</v>
+      </c>
+      <c r="B22" s="2">
+        <v>9</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A22" s="19">
-        <v>2.6</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>56</v>
-      </c>
       <c r="E22" s="10" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>60</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -1932,79 +2054,79 @@
         <v>2.6</v>
       </c>
       <c r="B23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>59</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A24" s="19">
         <v>2.6</v>
       </c>
       <c r="B24" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>59</v>
       </c>
       <c r="F24" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="19">
+        <v>2.6</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="20">
+    <row r="26" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="20">
         <v>2.7</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B26" s="2">
         <v>1</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C26" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D26" s="18" t="s">
         <v>72</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="21">
-        <v>2.7</v>
-      </c>
-      <c r="B26" s="2">
-        <v>2</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>73</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>74</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>76</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2012,359 +2134,363 @@
         <v>2.7</v>
       </c>
       <c r="B27" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
-        <v>87</v>
+      <c r="F27" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="21">
+        <v>2.7</v>
       </c>
       <c r="B28" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>84</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B29" s="2">
-        <v>2</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="18" t="s">
+      <c r="D30" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="F30" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="2">
-        <v>3</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B31" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>86</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="F31" s="38"/>
     </row>
     <row r="32" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B32" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F32" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B33" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F33" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="F33" s="39"/>
     </row>
     <row r="34" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B34" s="2">
+        <v>6</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="39"/>
+    </row>
+    <row r="35" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="2">
         <v>7</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C35" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" s="39"/>
+    </row>
+    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
-      <c r="C35" s="18" t="s">
+      <c r="D36" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="2">
-        <v>2</v>
-      </c>
-      <c r="C36" s="18" t="s">
+      <c r="F36" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2</v>
+      </c>
+      <c r="C37" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="2">
-        <v>3</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>104</v>
-      </c>
       <c r="D37" s="18" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="E37" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B38" s="2">
         <v>3</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="F38" s="39"/>
+    </row>
+    <row r="39" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B39" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F39" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B40" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F40" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="F40" s="39"/>
     </row>
     <row r="41" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B41" s="2">
+        <v>5</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" s="39"/>
+    </row>
+    <row r="42" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="2">
         <v>6</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C42" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" s="39"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="24">
+        <v>3.1</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="24">
+      <c r="D43" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="25">
         <v>3.1</v>
       </c>
-      <c r="B42" s="2">
-        <v>1</v>
-      </c>
-      <c r="C42" s="18" t="s">
+      <c r="B44" s="2">
+        <v>2</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="24">
+        <v>3.1</v>
+      </c>
+      <c r="B45" s="2">
+        <v>3</v>
+      </c>
+      <c r="C45" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D42" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F42" s="7" t="s">
+      <c r="D45" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" s="10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="25">
-        <v>3.1</v>
-      </c>
-      <c r="B43" s="2">
-        <v>2</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="24">
-        <v>3.1</v>
-      </c>
-      <c r="B44" s="2">
-        <v>3</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="26">
-        <v>3.2</v>
-      </c>
-      <c r="B45" s="2">
-        <v>1</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="F45" s="7" t="s">
-        <v>121</v>
+        <v>262</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2372,19 +2498,19 @@
         <v>3.2</v>
       </c>
       <c r="B46" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="F46" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2392,19 +2518,19 @@
         <v>3.2</v>
       </c>
       <c r="B47" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E47" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2412,745 +2538,777 @@
         <v>3.2</v>
       </c>
       <c r="B48" s="2">
+        <v>3</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A49" s="26">
+        <v>3.2</v>
+      </c>
+      <c r="B49" s="2">
         <v>4</v>
       </c>
-      <c r="C48" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A49" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="B49" s="2">
-        <v>1</v>
-      </c>
       <c r="C49" s="18" t="s">
-        <v>126</v>
+        <v>240</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>132</v>
+        <v>269</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="27" t="s">
-        <v>147</v>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A50" s="26">
+        <v>3.2</v>
       </c>
       <c r="B50" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>127</v>
+        <v>267</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>133</v>
+        <v>268</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>142</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F50" s="39"/>
     </row>
     <row r="51" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A51" s="27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B51" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F51" s="7"/>
+        <v>136</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A52" s="27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B52" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>246</v>
+        <v>125</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>247</v>
+        <v>131</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F52" s="7"/>
+        <v>136</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A53" s="27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B53" s="2">
+        <v>3</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="2">
+        <v>4</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A55" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="2">
         <v>5</v>
       </c>
-      <c r="C53" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F53" s="7"/>
-    </row>
-    <row r="54" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="B54" s="2">
-        <v>1</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A55" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="B55" s="2">
-        <v>2</v>
-      </c>
       <c r="C55" s="18" t="s">
-        <v>129</v>
+        <v>274</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>135</v>
+        <v>243</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>144</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A56" s="28" t="s">
-        <v>148</v>
+      <c r="A56" s="27" t="s">
+        <v>145</v>
       </c>
       <c r="B56" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>152</v>
+        <v>275</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>153</v>
+        <v>276</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F56" s="7"/>
+        <v>136</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A57" s="29" t="s">
-        <v>149</v>
+      <c r="A57" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="B57" s="2">
         <v>1</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="29" t="s">
-        <v>149</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A58" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="B58" s="2">
         <v>2</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D58" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="E58" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E58" s="10" t="s">
-        <v>140</v>
-      </c>
       <c r="F58" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="28" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A59" s="29" t="s">
-        <v>149</v>
       </c>
       <c r="B59" s="2">
         <v>3</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F59" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A60" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B60" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>253</v>
+        <v>134</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F60" s="7"/>
+        <v>138</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A61" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B61" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>251</v>
+        <v>129</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>254</v>
+        <v>135</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F61" s="7"/>
+        <v>138</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A62" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B62" s="2">
+        <v>3</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A63" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="2">
+        <v>4</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A64" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B64" s="2">
+        <v>5</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A65" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" s="2">
         <v>6</v>
       </c>
-      <c r="C62" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A63" s="30">
-        <v>4.3</v>
-      </c>
-      <c r="B63" s="2">
-        <v>1</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="D63" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="30">
-        <v>4.3</v>
-      </c>
-      <c r="B64" s="2">
-        <v>2</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A65" s="30">
-        <v>4.3</v>
-      </c>
-      <c r="B65" s="2">
-        <v>3</v>
-      </c>
       <c r="C65" s="18" t="s">
-        <v>157</v>
+        <v>246</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>161</v>
+        <v>249</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A66" s="30">
         <v>4.3</v>
       </c>
       <c r="B66" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D66" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E66" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A67" s="30">
         <v>4.3</v>
       </c>
       <c r="B67" s="2">
+        <v>2</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A68" s="30">
+        <v>4.3</v>
+      </c>
+      <c r="B68" s="2">
+        <v>3</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="30">
+        <v>4.3</v>
+      </c>
+      <c r="B69" s="2">
+        <v>4</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A70" s="30">
+        <v>4.3</v>
+      </c>
+      <c r="B70" s="2">
         <v>5</v>
       </c>
-      <c r="C67" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="E67" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="F67" s="7"/>
-    </row>
-    <row r="68" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="31">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B68" s="2">
-        <v>1</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="31">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B69" s="2">
-        <v>2</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="D69" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A70" s="31">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B70" s="2">
-        <v>3</v>
-      </c>
       <c r="C70" s="18" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F70" s="7"/>
-    </row>
-    <row r="71" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A71" s="31">
         <v>4.4000000000000004</v>
       </c>
       <c r="B71" s="2">
+        <v>1</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B72" s="2">
+        <v>2</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B73" s="2">
+        <v>3</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A74" s="31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B74" s="2">
         <v>4</v>
       </c>
-      <c r="C71" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F71" s="7"/>
-    </row>
-    <row r="72" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="32">
-        <v>4.5</v>
-      </c>
-      <c r="B72" s="2">
-        <v>1</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="32">
-        <v>4.5</v>
-      </c>
-      <c r="B73" s="2">
-        <v>2</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="32">
-        <v>4.5</v>
-      </c>
-      <c r="B74" s="2">
-        <v>3</v>
-      </c>
       <c r="C74" s="18" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F74" s="7"/>
-    </row>
-    <row r="75" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A75" s="32">
         <v>4.5</v>
       </c>
       <c r="B75" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F75" s="7"/>
+        <v>179</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="76" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A76" s="32">
         <v>4.5</v>
       </c>
       <c r="B76" s="2">
+        <v>2</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A77" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="B77" s="2">
+        <v>3</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A78" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="B78" s="2">
+        <v>4</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="B79" s="2">
         <v>5</v>
       </c>
-      <c r="C76" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="D76" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="E76" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F76" s="7"/>
-    </row>
-    <row r="77" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A77" s="33">
+      <c r="C79" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="33">
         <v>4.5999999999999996</v>
-      </c>
-      <c r="B77" s="2">
-        <v>1</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="D77" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A78" s="33">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="B78" s="2">
-        <v>2</v>
-      </c>
-      <c r="C78" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="D78" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A79" s="33">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="B79" s="2">
-        <v>3</v>
-      </c>
-      <c r="C79" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="D79" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="F79" s="7"/>
-    </row>
-    <row r="80" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A80" s="34">
-        <v>5.0999999999999996</v>
       </c>
       <c r="B80" s="2">
         <v>1</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A81" s="34">
-        <v>5.0999999999999996</v>
+      <c r="A81" s="33">
+        <v>4.5999999999999996</v>
       </c>
       <c r="B81" s="2">
         <v>2</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F81" s="7"/>
-    </row>
-    <row r="82" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A82" s="34">
-        <v>5.0999999999999996</v>
+        <v>196</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A82" s="33">
+        <v>4.5999999999999996</v>
       </c>
       <c r="B82" s="2">
         <v>3</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A83" s="34">
         <v>5.0999999999999996</v>
       </c>
       <c r="B83" s="2">
+        <v>1</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="34">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B84" s="2">
+        <v>2</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A85" s="34">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B85" s="2">
+        <v>3</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A86" s="34">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B86" s="2">
         <v>4</v>
       </c>
-      <c r="C83" s="18" t="s">
+      <c r="C86" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D86" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="D83" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="E83" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A84" s="35">
-        <v>6.2</v>
-      </c>
-      <c r="B84" s="2">
-        <v>1</v>
-      </c>
-      <c r="C84" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="D84" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="E84" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A85" s="35">
-        <v>6.2</v>
-      </c>
-      <c r="B85" s="2">
-        <v>2</v>
-      </c>
-      <c r="C85" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A86" s="35">
-        <v>6.2</v>
-      </c>
-      <c r="B86" s="2">
-        <v>3</v>
-      </c>
-      <c r="C86" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="D86" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="E86" s="10" t="s">
-        <v>214</v>
+        <v>137</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>217</v>
+        <v>288</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3158,224 +3316,279 @@
         <v>6.2</v>
       </c>
       <c r="B87" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="F87" s="7"/>
+        <v>211</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="88" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A88" s="35">
         <v>6.2</v>
       </c>
       <c r="B88" s="2">
+        <v>2</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A89" s="35">
+        <v>6.2</v>
+      </c>
+      <c r="B89" s="2">
+        <v>3</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A90" s="35">
+        <v>6.2</v>
+      </c>
+      <c r="B90" s="2">
+        <v>4</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A91" s="35">
+        <v>6.2</v>
+      </c>
+      <c r="B91" s="2">
         <v>5</v>
       </c>
-      <c r="C88" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="D88" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="F88" s="7"/>
-    </row>
-    <row r="89" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A89" s="36">
+      <c r="C91" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A92" s="36">
         <v>7</v>
-      </c>
-      <c r="B89" s="2">
-        <v>1</v>
-      </c>
-      <c r="C89" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="D89" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E89" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A90" s="36">
-        <v>7</v>
-      </c>
-      <c r="B90" s="2">
-        <v>2</v>
-      </c>
-      <c r="C90" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="D90" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="E90" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="36">
-        <v>7</v>
-      </c>
-      <c r="B91" s="2">
-        <v>2</v>
-      </c>
-      <c r="C91" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="D91" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="E91" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="F91" s="7"/>
-    </row>
-    <row r="92" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A92" s="37">
-        <v>8</v>
       </c>
       <c r="B92" s="2">
         <v>1</v>
       </c>
       <c r="C92" s="18" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A93" s="37">
-        <v>8</v>
+      <c r="A93" s="36">
+        <v>7</v>
       </c>
       <c r="B93" s="2">
         <v>2</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E93" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A94" s="36">
+        <v>7</v>
+      </c>
+      <c r="B94" s="2">
+        <v>2</v>
+      </c>
+      <c r="C94" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="F93" s="7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="37">
-        <v>8</v>
-      </c>
-      <c r="B94" s="2">
-        <v>3</v>
-      </c>
-      <c r="C94" s="18" t="s">
-        <v>229</v>
-      </c>
       <c r="D94" s="18" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+      <c r="F94" s="39"/>
+    </row>
+    <row r="95" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A95" s="37">
         <v>8</v>
       </c>
       <c r="B95" s="2">
+        <v>1</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A96" s="37">
+        <v>8</v>
+      </c>
+      <c r="B96" s="2">
+        <v>2</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A97" s="37">
+        <v>8</v>
+      </c>
+      <c r="B97" s="2">
+        <v>3</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A98" s="37">
+        <v>8</v>
+      </c>
+      <c r="B98" s="2">
         <v>4</v>
       </c>
-      <c r="C95" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="D95" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="F95" s="7" t="s">
+      <c r="C98" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="D98" s="18" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F96" s="7"/>
-    </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F97" s="7"/>
-    </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F98" s="7"/>
-    </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="E98" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F111" s="7"/>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F112" s="7"/>
     </row>
     <row r="113" spans="6:6" x14ac:dyDescent="0.2">
@@ -3867,7 +4080,17 @@
     <row r="275" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F275" s="7"/>
     </row>
+    <row r="276" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F276" s="7"/>
+    </row>
+    <row r="277" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F277" s="7"/>
+    </row>
+    <row r="278" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F278" s="7"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F98"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add support for rules of store and acc test checking it
</commit_message>
<xml_diff>
--- a/doc/ver1_fixes/AcceptanceTests - New.xlsx
+++ b/doc/ver1_fixes/AcceptanceTests - New.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="291">
   <si>
     <t>use case</t>
   </si>
@@ -905,6 +905,9 @@
   </si>
   <si>
     <t>משתמש אשר מזוהה כמנהל מערכת מנסה להסיר משתמש אשר לא קיים במערכת id_1</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore5()</t>
   </si>
 </sst>
 </file>
@@ -1594,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F278"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2589,7 +2592,9 @@
       <c r="E50" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F50" s="39"/>
+      <c r="F50" s="7" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A51" s="27" t="s">

</xml_diff>

<commit_message>
almost finished alternating immediate buy
</commit_message>
<xml_diff>
--- a/doc/ver1_fixes/AcceptanceTests - New.xlsx
+++ b/doc/ver1_fixes/AcceptanceTests - New.xlsx
@@ -1597,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F278"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finish fixing immediate buy cenrio
</commit_message>
<xml_diff>
--- a/doc/ver1_fixes/AcceptanceTests - New.xlsx
+++ b/doc/ver1_fixes/AcceptanceTests - New.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$99</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="299">
   <si>
     <t>use case</t>
   </si>
@@ -281,640 +281,664 @@
     <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #buySingleItem</t>
   </si>
   <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem1_only_buy_step()
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem2_only_buy_step()</t>
+  </si>
+  <si>
+    <t>2.8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום ופרטי אספקה </t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש רוצה לקנות מוצר אחד Id_1 אשר לא קיים במערכת, מזין פרטי תשלום ופרטי אספקה </t>
+  </si>
+  <si>
+    <t>המשתמש האורח רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום תקינים ופרטי אספקה שאינם תואמים את מדיניות הקנייה</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי ההזמנה לא עומדת במדיניות החנות והרכישה לא התבצעה</t>
+  </si>
+  <si>
+    <t>המשתמש רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום ופרטי אספקה אך מערכת הגבייה נפלה</t>
+  </si>
+  <si>
+    <t>המשתמש רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום ופרטי אספקה אך מערכת האספקה נפלה</t>
+  </si>
+  <si>
+    <t>המערכת הציגה סכום לתשלום אך מודיעה שזמנית לא ניתן להשלים את ההזמנה.</t>
+  </si>
+  <si>
+    <t>2.8.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות בקנייה, מזין פרטי תשלום ופרטי אספקה </t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות כאשר לא כולם קיימים במערכת, מזין פרטי תשלום ופרטי אספקה </t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #buyManyItems</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems3()</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי אין את הפריטים הרצוים במלאי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות כאשר כולם קיימים במערכת אך חלקם לא זמינים במלאי, מזין פרטי תשלום ופרטי אספקה </t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות, מזין פרטי תשלום שגוים ופרטי אספקה </t>
+  </si>
+  <si>
+    <t>המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות, מזין פרטי תשלום תקינים ופרטי אספקה שאינם תואמים את מדיניות הקנייה</t>
+  </si>
+  <si>
+    <t>המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות, מזין פרטי תשלום ופרטי אספקה אך מערכת הגבייה נפלה</t>
+  </si>
+  <si>
+    <t>המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות, מזין פרטי תשלום ופרטי אספקה אך מערכת האספקה נפלה</t>
+  </si>
+  <si>
+    <t>המשתמש לא מחובר למערכת</t>
+  </si>
+  <si>
+    <t>המשתמש מנוי ומחובר למערכת</t>
+  </si>
+  <si>
+    <t>המשתמש מנוי ולא מחובר למערכת</t>
+  </si>
+  <si>
+    <t>המשתמש אורח</t>
+  </si>
+  <si>
+    <t>המערכת מציגה הודעה כי אורחים לא יכולים להתנתק מהמערכת</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_logout1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_logout2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #logout</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אשר לא קיימת במערכת</t>
+  </si>
+  <si>
+    <t>המשתמש לא מזוהה כמנוי של המערכת. הוא מבקש לפתוח את החנות id_1</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אשר קיימת כבר במערכת</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #addStore</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore3()</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שכדי לפתוח חנות המשתמש חייב להיות מנוי של המערכת. לא נפתחת חנות id_1</t>
+  </si>
+  <si>
+    <t>נפתחה החנות id_1. המשתמש מוגדר כבעל חנות</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מוסיף את המוצר id_1 אשר לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המשתמש אינו מזוהה כבעל החנות. הוא מנסה להוסיף את המוצר id_1 אשר לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מסיר את המוצר id_1 אשר קיים בחנות</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מסיר את המוצר id_1 אשר לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות</t>
+  </si>
+  <si>
+    <t>המשתמש אינו מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות</t>
+  </si>
+  <si>
+    <t>המוצר הוסף בהצלחה לחנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שעל מנת להוסיף מוצר לחנות חייב המשתמש להיות בעל הרשאות. המוצר id_1 לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המוצר id_1 מוסר מהחנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שהמוצר לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המוצר id_1 נערך בהצלחה</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שעל מנת לערוך מוצר מהחנות חייב המשתמש להיות בעל הרשאות. המוצר id_1 נותר ללא שינוי</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #addItemToStore</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #removeItemFromStore</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #changeItemInStore</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeItemFromStore1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeItemFromStore2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore2()</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר אשר כבר קיים בחנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעת שגיאה שכן מוצר הוא ייחודי בחנות.</t>
+  </si>
+  <si>
+    <t>המשתמש אינו מזוהה כבעל החנות. הוא מסיר את המוצר id_1 אשר קיים בחנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שעל מנת להסיר מוצר לחנות חייב המשתמש להיות בעל הרשאות. המוצר id_1 נותר בחנות.</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מנסה לערוך את המוצר id_1 אשר לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי. יש ממנה יחיד לחנות</t>
+  </si>
+  <si>
+    <t>משתמש לא מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי. יש ממנה יחיד לחנות שזהותו id_2</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים למנות לא מזוהה כמנוי</t>
+  </si>
+  <si>
+    <t>משתמש id_1 מזוהה כבעל חנות אשר מונה על ידי משתמש id_2. המשתמש id_2 מנסה למנות לבעל החנות את Id_1</t>
+  </si>
+  <si>
+    <t>מנוי id_1 נהפך לבעל חנות נוסף שיש לו זכויות לניהול החנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שרק בעל החנות יכול מנות להיות בעל חנות נוסף. Id_2 נותר בעל החנות היחידי</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שניתן להוסיף רק מנויים במערכת</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שבעל חנות לא יכול להוסיף את מי שהוסיף אותו (אין מעגליות)</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #addOwner</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner4()</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שרק בעל החנות אשר מינה את id_1 יכול להסיר אותו. Id_1 נותר בעל החנות</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #removeOwner</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner2()</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כבעל החנות אשר המשתמש מינה להיות בעל חנות</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כבעל החנות אשר לא המשתמש מינה להיות בעל חנות</t>
+  </si>
+  <si>
+    <t>משתמש אינו מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כבעל החנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שרק בעל החנות יכול להסיר בעל חנות</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר אינו מזוהה כבעל חנות.</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שניתן להסיר רק בעלי חנויות</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי, מבקשים הרשאה לערוך מוצרים. יש ממנה יחיד לחנות</t>
+  </si>
+  <si>
+    <t>מנוי id_1 נהפך למנהל חנות נוסף שיש לו זכויות לערוך מוצרי החנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שרק בעל החנות יכול למנות מנהל חנות נוסף. Id_2 נותר בעל החנות היחידי</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #addManager</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager2()</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים למנות כבר הינו בעל חנות. יש ממנה יחיד לחנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שניתן למנות מי שאינו בעל החנות</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות והמשתמש id_1 שאותו רוצים למנות מזוהה כבר כמנהל החנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שניתן למנות מי שאינו מנהל החנות</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות והמשתמש id_1 שאותו רוצים למנות אינו מזוהה כמנוי.</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שניתן למנות רק מנויים</t>
+  </si>
+  <si>
+    <t>משתמש id_1 מזוהה כמנהל חנות אשר מונה על ידי משתמש id_2. המשתמש id_1 מנסה למנות למנהל החנות את Id_2</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שמנהל חנות לא יכול להוסיף את מי שהוסיף אותו (אין מעגליות)</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כמנהל החנות אשר המשתמש מינה להיות בעל חנות</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כמנהל החנות אשר לא המשתמש מינה להיות בעל חנות</t>
+  </si>
+  <si>
+    <t>מנוי id_1 לא מוגדר כמנהל החנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שרק בעל החנות אשר מינה את id_1 יכול להסיר אותו. Id_1 נותר מנהל החנות</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeManager1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeManager2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #removeManager</t>
+  </si>
+  <si>
+    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר אינו מזוהה כמנהל חנות.</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על זה שניתן להסיר רק מנהלי חנויות</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנהל חנות אשר יש לו הרשאות להסיר מוצר ממלאי החנות מנסה להסיר מוצר ממלאי החנות</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנהל חנות אשר אין לו הרשאות להסיר מוצר ממלאי החנות מנסה להסיר מוצר ממלאי החנות</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנוי רגיל מנסה להסיר מוצר ממלאי החנות</t>
+  </si>
+  <si>
+    <t>המוצר מוסר ממלאי החנות</t>
+  </si>
+  <si>
+    <t>המערכת מציגה למשתמש הודעה על כך שעל מנת להסיר מוצר הוא צריך הרשאות להסרת מוצר. המוצר נותר במלאי</t>
+  </si>
+  <si>
+    <t>המערכת מציגה למשתמש הודעה על כך שרק מנהל חנות יכול להסיר מוצר. המוצר נותר במלאי</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeItemFromStore3()</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנהל חנות אשר יש לו הרשאות להסיר מוצר ממלאי החנות מנסה להסיר מהחנות מוצר שלא קיים</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה על שגיאה כי המוצר אינו קיים</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 (ולו אין קניות או מכירות בתהליך)</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 שהינו בעל חנות יחיד</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר לא קיים במערכת id_1</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #removeUser</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser1()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser3()</t>
+  </si>
+  <si>
+    <t>המשתמש id_1 מוסר מהמערכת</t>
+  </si>
+  <si>
+    <t>המשתמש id_1 מוסר מהמערכת וכן חנותו והמוצרים אותם הוא מוכר נמחקים מהמערכת</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעת שגיאה על כך שהמשתמש שאותו רוצים להסיר לא קיים במערכת</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעת שגיאה על כך שרק מנהל המערכת מורשה למחוק משתמשים</t>
+  </si>
+  <si>
+    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 שהינו בעל חנות שאינו יחיד</t>
+  </si>
+  <si>
+    <t>המשתמש id_1 מוסר מהמערכת והוא אינו בעל החנות יותר</t>
+  </si>
+  <si>
+    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות. כן, המשתמש הזין פרטי תשלום ולידיים.</t>
+  </si>
+  <si>
+    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות אך המשתמש הזין פרטי תשלום שאינם ולידיים</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה אישור כי העסקה בוצעה בהצלחה</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי התשלום נכשל ומציעה למשתמש להזין פרטי התשלום בשנית</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה אישור כי התקבלה הבקשה לאספקה וכן חוזר מספר משלוח</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעת שגיאה על כך שלא ניתן להזמין אספקה עבור כתובת זו ומציעה למשתמש להזין כתובת אחרת</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #pay</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #supply</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem1_only_pay_step()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem1_only_supply_step()</t>
+  </si>
+  <si>
+    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות. כן, המשתמש הזין פרטי תשלום ולידיים. מערכת הגבייה נפלה</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי התשלום נכשל ומציעה למשתמש לנסות מאוחר יותר</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אך תיאור החנות קצר מדי</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שמחירו שלילי.</t>
+  </si>
+  <si>
+    <t>המערכת מחווה כי מחיר מוצר חייב להיות חיובי. המוצר לא נוסף לחנות.</t>
+  </si>
+  <si>
+    <t>המערכת מחווה כי כמות מוצר חייבת להיות חיובית. המוצר לא נוסף לחנות.</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות ומזין מחיר חדש שלילי</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות ומזין כמות חדשה שאינה שלמה</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות ומזין שם חדש שאינו ייחודי לחנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שלא ניתן להזין מחיר שלילי למוצר</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שלא ניתן להזין כמות שאינה שלמה למוצר</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שהשם הנבחר כבר תפוס.</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_setup3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_setup4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_setup5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_login4()</t>
+  </si>
+  <si>
+    <t>חיפוש לפי שם מוצר ריק</t>
+  </si>
+  <si>
+    <t>המערכת תציג את כל המוצרים במערכת</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_searchItem7()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_searchItem8()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_searchItem9()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_watchCart()   test_removeItemFromCart</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemQuantityInCart()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemQuantityInCart2()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_logout3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore5()</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אך החוקים יוצרים סתירה</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי החוקים יוצרים סתירה. לא נפתחת חנות id_1</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי תיאור חנות צריך לכלול לפחות 20 תווים. לא נפתחת חנות id_1</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore6()</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שכמותו שלילית</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שכמותו אינה שלמה</t>
+  </si>
+  <si>
+    <t>המערכת מחווה כי כמות מוצר חייבת להיות שלמה. המוצר לא נוסף לחנות.</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore6()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager4()</t>
+  </si>
+  <si>
+    <t>מנוי id_1 לא מוגדר כבעל החנות וכל מי שהוא מינה אינם בעלי החנות גם כן</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeManager3()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeItemFromStore4()</t>
+  </si>
+  <si>
+    <t>משתמש אשר מזוהה כמנהל מערכת מנסה להסיר משתמש אשר לא קיים במערכת id_1</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore5()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש רוצה לקנות 2 פריטים ממוצר Id_1 אשר קיים במערכת אך קיים רק פריט אחד זמין במלאי. </t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem3_only_buy_step()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem4()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem5()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem6()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem7()</t>
+  </si>
+  <si>
+    <t>המשתמש האורח רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום תקינים אך פרטי אספקה לא תקינים</t>
+  </si>
+  <si>
+    <t>המערכת הציגה סכום לתשלום והמערכת מודיעה כי פרטי האספקה שגויים והרכישה לא התבצעה</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem8()</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem1_only_buy_step()   
 {$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem1_only_pay_step()
 {$gitRepo}\dev\AcceptanceTests\test_acc.py #test_test_buySingleItem1_only_supply_step()</t>
   </si>
   <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem2_only_buy_step()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem3()</t>
-  </si>
-  <si>
-    <t>2.8.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">המשתמש רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום ופרטי אספקה </t>
-  </si>
-  <si>
-    <t xml:space="preserve">המשתמש רוצה לקנות מוצר אחד Id_1 אשר לא קיים במערכת, מזין פרטי תשלום ופרטי אספקה </t>
-  </si>
-  <si>
-    <t>המשתמש האורח רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום תקינים ופרטי אספקה שאינם תואמים את מדיניות הקנייה</t>
-  </si>
-  <si>
-    <t>המערכת מודיעה כי ההזמנה לא עומדת במדיניות החנות והרכישה לא התבצעה</t>
-  </si>
-  <si>
-    <t>המשתמש רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום ופרטי אספקה אך מערכת הגבייה נפלה</t>
-  </si>
-  <si>
-    <t>המשתמש רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום ופרטי אספקה אך מערכת האספקה נפלה</t>
-  </si>
-  <si>
-    <t>המערכת הציגה סכום לתשלום אך מודיעה שזמנית לא ניתן להשלים את ההזמנה.</t>
-  </si>
-  <si>
-    <t>2.8.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות בקנייה, מזין פרטי תשלום ופרטי אספקה </t>
-  </si>
-  <si>
-    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות כאשר לא כולם קיימים במערכת, מזין פרטי תשלום ופרטי אספקה </t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #buyManyItems</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems3()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">המשתמש רוצה לקנות 2 פריטים ממוצר Id_1 אשר קיים במערכת אך קיים רק פריט אחד זמין במלאי. המשתמש מזין פרטי תשלום ופרטי אספקה </t>
-  </si>
-  <si>
-    <t>המערכת מודיעה כי אין את הפריטים הרצוים במלאי</t>
-  </si>
-  <si>
-    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות כאשר כולם קיימים במערכת אך חלקם לא זמינים במלאי, מזין פרטי תשלום ופרטי אספקה </t>
-  </si>
-  <si>
-    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות, מזין פרטי תשלום שגוים ופרטי אספקה </t>
-  </si>
-  <si>
-    <t>המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות, מזין פרטי תשלום תקינים ופרטי אספקה שאינם תואמים את מדיניות הקנייה</t>
-  </si>
-  <si>
-    <t>המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות, מזין פרטי תשלום ופרטי אספקה אך מערכת הגבייה נפלה</t>
-  </si>
-  <si>
-    <t>המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות, מזין פרטי תשלום ופרטי אספקה אך מערכת האספקה נפלה</t>
-  </si>
-  <si>
-    <t>המשתמש לא מחובר למערכת</t>
-  </si>
-  <si>
-    <t>המשתמש מנוי ומחובר למערכת</t>
-  </si>
-  <si>
-    <t>המשתמש מנוי ולא מחובר למערכת</t>
-  </si>
-  <si>
-    <t>המשתמש אורח</t>
-  </si>
-  <si>
-    <t>המערכת מציגה הודעה כי אורחים לא יכולים להתנתק מהמערכת</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_logout1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_logout2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #logout</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אשר לא קיימת במערכת</t>
-  </si>
-  <si>
-    <t>המשתמש לא מזוהה כמנוי של המערכת. הוא מבקש לפתוח את החנות id_1</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אשר קיימת כבר במערכת</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #addStore</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore3()</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שכדי לפתוח חנות המשתמש חייב להיות מנוי של המערכת. לא נפתחת חנות id_1</t>
-  </si>
-  <si>
-    <t>נפתחה החנות id_1. המשתמש מוגדר כבעל חנות</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא מוסיף את המוצר id_1 אשר לא קיים בחנות</t>
-  </si>
-  <si>
-    <t>המשתמש אינו מזוהה כבעל החנות. הוא מנסה להוסיף את המוצר id_1 אשר לא קיים בחנות</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא מסיר את המוצר id_1 אשר קיים בחנות</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא מסיר את המוצר id_1 אשר לא קיים בחנות</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות</t>
-  </si>
-  <si>
-    <t>המשתמש אינו מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות</t>
-  </si>
-  <si>
-    <t>המוצר הוסף בהצלחה לחנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שעל מנת להוסיף מוצר לחנות חייב המשתמש להיות בעל הרשאות. המוצר id_1 לא קיים בחנות</t>
-  </si>
-  <si>
-    <t>המוצר id_1 מוסר מהחנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שהמוצר לא קיים בחנות</t>
-  </si>
-  <si>
-    <t>המוצר id_1 נערך בהצלחה</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שעל מנת לערוך מוצר מהחנות חייב המשתמש להיות בעל הרשאות. המוצר id_1 נותר ללא שינוי</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #addItemToStore</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #removeItemFromStore</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #changeItemInStore</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeItemFromStore1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeItemFromStore2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore2()</t>
-  </si>
-  <si>
-    <t>4.1.1</t>
-  </si>
-  <si>
-    <t>4.1.2</t>
-  </si>
-  <si>
-    <t>4.1.3</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר אשר כבר קיים בחנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעת שגיאה שכן מוצר הוא ייחודי בחנות.</t>
-  </si>
-  <si>
-    <t>המשתמש אינו מזוהה כבעל החנות. הוא מסיר את המוצר id_1 אשר קיים בחנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שעל מנת להסיר מוצר לחנות חייב המשתמש להיות בעל הרשאות. המוצר id_1 נותר בחנות.</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא מנסה לערוך את המוצר id_1 אשר לא קיים בחנות</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי. יש ממנה יחיד לחנות</t>
-  </si>
-  <si>
-    <t>משתמש לא מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי. יש ממנה יחיד לחנות שזהותו id_2</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים למנות לא מזוהה כמנוי</t>
-  </si>
-  <si>
-    <t>משתמש id_1 מזוהה כבעל חנות אשר מונה על ידי משתמש id_2. המשתמש id_2 מנסה למנות לבעל החנות את Id_1</t>
-  </si>
-  <si>
-    <t>מנוי id_1 נהפך לבעל חנות נוסף שיש לו זכויות לניהול החנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שרק בעל החנות יכול מנות להיות בעל חנות נוסף. Id_2 נותר בעל החנות היחידי</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שניתן להוסיף רק מנויים במערכת</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שבעל חנות לא יכול להוסיף את מי שהוסיף אותו (אין מעגליות)</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #addOwner</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner3()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner4()</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שרק בעל החנות אשר מינה את id_1 יכול להסיר אותו. Id_1 נותר בעל החנות</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #removeOwner</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner2()</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כבעל החנות אשר המשתמש מינה להיות בעל חנות</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כבעל החנות אשר לא המשתמש מינה להיות בעל חנות</t>
-  </si>
-  <si>
-    <t>משתמש אינו מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כבעל החנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שרק בעל החנות יכול להסיר בעל חנות</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר אינו מזוהה כבעל חנות.</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שניתן להסיר רק בעלי חנויות</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי, מבקשים הרשאה לערוך מוצרים. יש ממנה יחיד לחנות</t>
-  </si>
-  <si>
-    <t>מנוי id_1 נהפך למנהל חנות נוסף שיש לו זכויות לערוך מוצרי החנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שרק בעל החנות יכול למנות מנהל חנות נוסף. Id_2 נותר בעל החנות היחידי</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #addManager</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager2()</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים למנות כבר הינו בעל חנות. יש ממנה יחיד לחנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שניתן למנות מי שאינו בעל החנות</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות והמשתמש id_1 שאותו רוצים למנות מזוהה כבר כמנהל החנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שניתן למנות מי שאינו מנהל החנות</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות והמשתמש id_1 שאותו רוצים למנות אינו מזוהה כמנוי.</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שניתן למנות רק מנויים</t>
-  </si>
-  <si>
-    <t>משתמש id_1 מזוהה כמנהל חנות אשר מונה על ידי משתמש id_2. המשתמש id_1 מנסה למנות למנהל החנות את Id_2</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שמנהל חנות לא יכול להוסיף את מי שהוסיף אותו (אין מעגליות)</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כמנהל החנות אשר המשתמש מינה להיות בעל חנות</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר מזוהה כמנהל החנות אשר לא המשתמש מינה להיות בעל חנות</t>
-  </si>
-  <si>
-    <t>מנוי id_1 לא מוגדר כמנהל החנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שרק בעל החנות אשר מינה את id_1 יכול להסיר אותו. Id_1 נותר מנהל החנות</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeManager1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeManager2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #removeManager</t>
-  </si>
-  <si>
-    <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים להסיר אינו מזוהה כמנהל חנות.</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שניתן להסיר רק מנהלי חנויות</t>
-  </si>
-  <si>
-    <t>משתמש אשר רשום כמנהל חנות אשר יש לו הרשאות להסיר מוצר ממלאי החנות מנסה להסיר מוצר ממלאי החנות</t>
-  </si>
-  <si>
-    <t>משתמש אשר רשום כמנהל חנות אשר אין לו הרשאות להסיר מוצר ממלאי החנות מנסה להסיר מוצר ממלאי החנות</t>
-  </si>
-  <si>
-    <t>משתמש אשר רשום כמנוי רגיל מנסה להסיר מוצר ממלאי החנות</t>
-  </si>
-  <si>
-    <t>המוצר מוסר ממלאי החנות</t>
-  </si>
-  <si>
-    <t>המערכת מציגה למשתמש הודעה על כך שעל מנת להסיר מוצר הוא צריך הרשאות להסרת מוצר. המוצר נותר במלאי</t>
-  </si>
-  <si>
-    <t>המערכת מציגה למשתמש הודעה על כך שרק מנהל חנות יכול להסיר מוצר. המוצר נותר במלאי</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeItemFromStore3()</t>
-  </si>
-  <si>
-    <t>משתמש אשר רשום כמנהל חנות אשר יש לו הרשאות להסיר מוצר ממלאי החנות מנסה להסיר מהחנות מוצר שלא קיים</t>
-  </si>
-  <si>
-    <t>המערכת מודיעה על שגיאה כי המוצר אינו קיים</t>
-  </si>
-  <si>
-    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 (ולו אין קניות או מכירות בתהליך)</t>
-  </si>
-  <si>
-    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 שהינו בעל חנות יחיד</t>
-  </si>
-  <si>
-    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר לא קיים במערכת id_1</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #removeUser</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser3()</t>
-  </si>
-  <si>
-    <t>המשתמש id_1 מוסר מהמערכת</t>
-  </si>
-  <si>
-    <t>המשתמש id_1 מוסר מהמערכת וכן חנותו והמוצרים אותם הוא מוכר נמחקים מהמערכת</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעת שגיאה על כך שהמשתמש שאותו רוצים להסיר לא קיים במערכת</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעת שגיאה על כך שרק מנהל המערכת מורשה למחוק משתמשים</t>
-  </si>
-  <si>
-    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 שהינו בעל חנות שאינו יחיד</t>
-  </si>
-  <si>
-    <t>המשתמש id_1 מוסר מהמערכת והוא אינו בעל החנות יותר</t>
-  </si>
-  <si>
-    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות. כן, המשתמש הזין פרטי תשלום ולידיים.</t>
-  </si>
-  <si>
-    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות אך המשתמש הזין פרטי תשלום שאינם ולידיים</t>
-  </si>
-  <si>
-    <t>המשתמש מבקש להזמין אספקה עבור סל הקניות שלו על עסקה שקיים לה אישור תשלום ממערכת הגבייה</t>
-  </si>
-  <si>
-    <t>המשתמש מבקש להזמין אספקה עבור סל הקניות שלו על עסקה שקיים לה אישור תשלום ממערכת הגבייה אך מזין כתובת שחברת האספקה לא מספקת אליה</t>
-  </si>
-  <si>
-    <t>המשתמש מבקש להזמין אספקה עבור סל הקניות שלו על עסקה שלא אושר עליה תשלום ממערכת הגבייה</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה אישור כי העסקה בוצעה בהצלחה</t>
-  </si>
-  <si>
-    <t>המערכת מודיעה כי התשלום נכשל ומציעה למשתמש להזין פרטי התשלום בשנית</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה אישור כי התקבלה הבקשה לאספקה וכן חוזר מספר משלוח</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעת שגיאה על כך שלא ניתן להזמין אספקה עבור כתובת זו ומציעה למשתמש להזין כתובת אחרת</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעת שגיאה על כך שלא ניתן להזמין אספקה עבור סל קניות עליו אין אישור תשלום ממערכת הגבייה</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #pay</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #supply</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem1_only_pay_step()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem1_only_supply_step()</t>
-  </si>
-  <si>
-    <t>לא בר מימוש בגרסה זאת</t>
-  </si>
-  <si>
-    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות. כן, המשתמש הזין פרטי תשלום ולידיים. מערכת הגבייה נפלה</t>
-  </si>
-  <si>
-    <t>המערכת מודיעה כי התשלום נכשל ומציעה למשתמש לנסות מאוחר יותר</t>
-  </si>
-  <si>
-    <t>המשתמש מבקש להזמין אספקה עבור סל הקניות שלו על עסקה שקיים לה אישור תשלום ממערכת הגבייה אך מערכת האספקה נפלה</t>
-  </si>
-  <si>
-    <t>המערכת מודיעה כי האספקה נכשלה ומציעה למשתמש להזין פרטי התשלום בשנית. מתבצע זיכוי לחשבונו של הלקוח.</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אך תיאור החנות קצר מדי</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שמחירו שלילי.</t>
-  </si>
-  <si>
-    <t>המערכת מחווה כי מחיר מוצר חייב להיות חיובי. המוצר לא נוסף לחנות.</t>
-  </si>
-  <si>
-    <t>המערכת מחווה כי כמות מוצר חייבת להיות חיובית. המוצר לא נוסף לחנות.</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות ומזין מחיר חדש שלילי</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות ומזין כמות חדשה שאינה שלמה</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות ומזין שם חדש שאינו ייחודי לחנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שלא ניתן להזין מחיר שלילי למוצר</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שלא ניתן להזין כמות שאינה שלמה למוצר</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שהשם הנבחר כבר תפוס.</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_setup3()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_setup4()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_setup5()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_login4()</t>
-  </si>
-  <si>
-    <t>חיפוש לפי שם מוצר ריק</t>
-  </si>
-  <si>
-    <t>המערכת תציג את כל המוצרים במערכת</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_searchItem7()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_searchItem8()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_searchItem9()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_watchCart()   test_removeItemFromCart</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemQuantityInCart()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemQuantityInCart2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_logout3()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore4()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore3()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore4()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore5()</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כמנוי של המערכת והוא מבקש לפתוח את החנות id_1, אך החוקים יוצרים סתירה</t>
-  </si>
-  <si>
-    <t>המערכת מודיעה כי החוקים יוצרים סתירה. לא נפתחת חנות id_1</t>
-  </si>
-  <si>
-    <t>המערכת מודיעה כי תיאור חנות צריך לכלול לפחות 20 תווים. לא נפתחת חנות id_1</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore3()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore4()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore5()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_changeItemInStore6()</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שכמותו שלילית</t>
-  </si>
-  <si>
-    <t>המשתמש מזוהה כבעל החנות. הוא מנסה להוסיף מוצר שכמותו אינה שלמה</t>
-  </si>
-  <si>
-    <t>המערכת מחווה כי כמות מוצר חייבת להיות שלמה. המוצר לא נוסף לחנות.</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addItemToStore6()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addOwner5()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner3()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeOwner4()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager3()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager4()</t>
-  </si>
-  <si>
-    <t>מנוי id_1 לא מוגדר כבעל החנות וכל מי שהוא מינה אינם בעלי החנות גם כן</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addManager5()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeManager3()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser4()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeUser5()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_removeItemFromStore4()</t>
-  </si>
-  <si>
-    <t>משתמש אשר מזוהה כמנהל מערכת מנסה להסיר משתמש אשר לא קיים במערכת id_1</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_addStore5()</t>
+    <t>המשתמש מבקש לבצע לרכוש מוצרים והעסקה עומדת בחוקי המדיניות שהגדיר בעל החנות. כן, המשתמש הזין פרטי תשלום ולידיים אך לא התקבל אישור ממערכת האספקה</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי התשלום נכשל ולא התבצע חיוב.</t>
+  </si>
+  <si>
+    <t>המשתמש מבקש להזמין אספקה עבור רכישה שביצע</t>
+  </si>
+  <si>
+    <t>המשתמש מבקש להזמין אספקה עבור רכישה ביצע אך מערכת האספקה נפלה</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי האספקה נכשלה ומציעה למשתמש לנסות שוב מאוחר יותר</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem9()</t>
+  </si>
+  <si>
+    <t>המשתמש מבקש להזמין אספקה עבור רכישה שביצע אך מזין כתובת שחברת האספקה לא מספקת אליה (מדיניות קניה)</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem10()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -929,12 +953,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FFFFC66D"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="28">
@@ -1150,7 +1168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1259,9 +1277,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1595,10 +1610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F278"/>
+  <dimension ref="A1:F279"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1608,7 +1623,7 @@
     <col min="3" max="3" width="42.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="53.25" style="2" customWidth="1"/>
     <col min="5" max="5" width="57" style="2" customWidth="1"/>
-    <col min="6" max="6" width="57.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="62.75" style="2" customWidth="1"/>
     <col min="7" max="16384" width="8.75" style="2"/>
   </cols>
   <sheetData>
@@ -1689,7 +1704,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1709,7 +1724,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1729,7 +1744,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1869,7 +1884,7 @@
         <v>29</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -1900,10 +1915,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>47</v>
@@ -2009,7 +2024,7 @@
         <v>47</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2029,7 +2044,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2049,7 +2064,7 @@
         <v>47</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -2129,7 +2144,7 @@
         <v>74</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2149,7 +2164,7 @@
         <v>74</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2169,18 +2184,18 @@
         <v>74</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>78</v>
@@ -2188,19 +2203,19 @@
       <c r="E29" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="F29" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B30" s="2">
         <v>2</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>79</v>
@@ -2209,311 +2224,319 @@
         <v>81</v>
       </c>
       <c r="F30" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="22" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="22" t="s">
-        <v>85</v>
       </c>
       <c r="B31" s="2">
         <v>3</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>100</v>
+        <v>281</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F31" s="38"/>
+      <c r="F31" s="7" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B32" s="2">
         <v>4</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>77</v>
+        <v>287</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>80</v>
+        <v>288</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>81</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>84</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B33" s="2">
         <v>5</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="7" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" s="2">
         <v>6</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="7" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B35" s="2">
         <v>7</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F35" s="39"/>
-    </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
-        <v>93</v>
+      <c r="F35" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="B36" s="2">
+        <v>8</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="2">
         <v>1</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C37" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" s="2">
-        <v>2</v>
-      </c>
-      <c r="C37" s="18" t="s">
+      <c r="F37" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2</v>
+      </c>
+      <c r="C38" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="2">
-        <v>3</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>102</v>
-      </c>
       <c r="D38" s="18" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E38" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F38" s="39"/>
-    </row>
-    <row r="39" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B39" s="2">
         <v>3</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D39" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="38"/>
+    </row>
+    <row r="40" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="2">
+        <v>3</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E39" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="B40" s="2">
-        <v>4</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>89</v>
-      </c>
       <c r="E40" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F40" s="39"/>
+        <v>94</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B41" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F41" s="39"/>
+        <v>94</v>
+      </c>
+      <c r="F41" s="38"/>
     </row>
     <row r="42" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B42" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>80</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F42" s="39"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="24">
+        <v>94</v>
+      </c>
+      <c r="F42" s="38"/>
+    </row>
+    <row r="43" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="2">
+        <v>6</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="38"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="24">
         <v>3.1</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B44" s="2">
         <v>1</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C44" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="25">
+        <v>3.1</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="24">
+        <v>3.1</v>
+      </c>
+      <c r="B46" s="2">
+        <v>3</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D43" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="25">
-        <v>3.1</v>
-      </c>
-      <c r="B44" s="2">
-        <v>2</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="24">
-        <v>3.1</v>
-      </c>
-      <c r="B45" s="2">
-        <v>3</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" s="18" t="s">
+      <c r="E46" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E45" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="26">
-        <v>3.2</v>
-      </c>
-      <c r="B46" s="2">
-        <v>1</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>118</v>
-      </c>
       <c r="F46" s="7" t="s">
-        <v>119</v>
+        <v>252</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2521,19 +2544,19 @@
         <v>3.2</v>
       </c>
       <c r="B47" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2541,19 +2564,19 @@
         <v>3.2</v>
       </c>
       <c r="B48" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2561,19 +2584,19 @@
         <v>3.2</v>
       </c>
       <c r="B49" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>240</v>
+        <v>114</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>269</v>
+        <v>119</v>
       </c>
       <c r="E49" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2581,439 +2604,439 @@
         <v>3.2</v>
       </c>
       <c r="B50" s="2">
+        <v>4</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="26">
+        <v>3.2</v>
+      </c>
+      <c r="B51" s="2">
         <v>5</v>
       </c>
-      <c r="C50" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="B51" s="2">
-        <v>1</v>
-      </c>
       <c r="C51" s="18" t="s">
-        <v>124</v>
+        <v>257</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>130</v>
+        <v>258</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>139</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A52" s="27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B52" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E52" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F52" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A53" s="27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B53" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>264</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A54" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="2">
+        <v>3</v>
+      </c>
+      <c r="C54" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="B54" s="2">
-        <v>4</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>241</v>
-      </c>
       <c r="D54" s="18" t="s">
-        <v>242</v>
+        <v>146</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B55" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A56" s="27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B56" s="2">
+        <v>5</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A57" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="2">
         <v>6</v>
       </c>
-      <c r="C56" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A57" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="B57" s="2">
-        <v>1</v>
-      </c>
       <c r="C57" s="18" t="s">
-        <v>126</v>
+        <v>265</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>132</v>
+        <v>266</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>141</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A58" s="28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B58" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A59" s="28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B59" s="2">
+        <v>2</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A60" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="2">
         <v>3</v>
       </c>
-      <c r="C59" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A60" s="29" t="s">
+      <c r="C60" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="B60" s="2">
-        <v>1</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>128</v>
-      </c>
       <c r="D60" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E60" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E60" s="10" t="s">
-        <v>138</v>
-      </c>
       <c r="F60" s="7" t="s">
-        <v>143</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A61" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B61" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D61" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E61" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="E61" s="10" t="s">
-        <v>138</v>
-      </c>
       <c r="F61" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A62" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B62" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>270</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A63" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B63" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>244</v>
+        <v>149</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>247</v>
+        <v>130</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A64" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B64" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A65" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B65" s="2">
+        <v>5</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A66" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="2">
         <v>6</v>
       </c>
-      <c r="C65" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A66" s="30">
-        <v>4.3</v>
-      </c>
-      <c r="B66" s="2">
-        <v>1</v>
-      </c>
       <c r="C66" s="18" t="s">
-        <v>153</v>
+        <v>236</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A67" s="30">
         <v>4.3</v>
       </c>
       <c r="B67" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D67" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="E67" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="E67" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="F67" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A68" s="30">
         <v>4.3</v>
       </c>
       <c r="B68" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C68" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D68" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="D68" s="18" t="s">
-        <v>159</v>
-      </c>
       <c r="E68" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A69" s="30">
         <v>4.3</v>
       </c>
       <c r="B69" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D69" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="D69" s="18" t="s">
-        <v>160</v>
-      </c>
       <c r="E69" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F69" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F69" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A70" s="30">
         <v>4.3</v>
       </c>
       <c r="B70" s="2">
+        <v>4</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A71" s="30">
+        <v>4.3</v>
+      </c>
+      <c r="B71" s="2">
         <v>5</v>
       </c>
-      <c r="C70" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="31">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B71" s="2">
-        <v>1</v>
-      </c>
       <c r="C71" s="18" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>283</v>
+        <v>180</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>168</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3021,39 +3044,39 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B72" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>166</v>
+        <v>273</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A73" s="31">
         <v>4.4000000000000004</v>
       </c>
       <c r="B73" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>279</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3061,39 +3084,39 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B74" s="2">
+        <v>3</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A75" s="31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B75" s="2">
         <v>4</v>
       </c>
-      <c r="C74" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="D74" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="32">
-        <v>4.5</v>
-      </c>
-      <c r="B75" s="2">
-        <v>1</v>
-      </c>
       <c r="C75" s="18" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3101,39 +3124,39 @@
         <v>4.5</v>
       </c>
       <c r="B76" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A77" s="32">
         <v>4.5</v>
       </c>
       <c r="B77" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>281</v>
+        <v>178</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3141,59 +3164,59 @@
         <v>4.5</v>
       </c>
       <c r="B78" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A79" s="32">
         <v>4.5</v>
       </c>
       <c r="B79" s="2">
+        <v>4</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="B80" s="2">
         <v>5</v>
       </c>
-      <c r="C79" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="D79" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A80" s="33">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="B80" s="2">
-        <v>1</v>
-      </c>
       <c r="C80" s="18" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>194</v>
+        <v>274</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3201,59 +3224,59 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="B81" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C81" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="F81" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D81" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A82" s="33">
         <v>4.5999999999999996</v>
       </c>
       <c r="B82" s="2">
+        <v>2</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A83" s="33">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B83" s="2">
         <v>3</v>
       </c>
-      <c r="C82" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="D82" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="E82" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A83" s="34">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B83" s="2">
-        <v>1</v>
-      </c>
       <c r="C83" s="18" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>141</v>
+        <v>275</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3261,19 +3284,19 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B84" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3281,59 +3304,59 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B85" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A86" s="34">
         <v>5.0999999999999996</v>
       </c>
       <c r="B86" s="2">
+        <v>3</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A87" s="34">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B87" s="2">
         <v>4</v>
       </c>
-      <c r="C86" s="18" t="s">
+      <c r="C87" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="D87" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="D86" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="E86" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F86" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A87" s="35">
-        <v>6.2</v>
-      </c>
-      <c r="B87" s="2">
-        <v>1</v>
-      </c>
-      <c r="C87" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="D87" s="18" t="s">
-        <v>215</v>
-      </c>
       <c r="E87" s="10" t="s">
-        <v>211</v>
+        <v>134</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>212</v>
+        <v>278</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3341,19 +3364,19 @@
         <v>6.2</v>
       </c>
       <c r="B88" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C88" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F88" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="D88" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3361,19 +3384,19 @@
         <v>6.2</v>
       </c>
       <c r="B89" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="D89" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="E89" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3381,19 +3404,19 @@
         <v>6.2</v>
       </c>
       <c r="B90" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>289</v>
+        <v>207</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E90" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F90" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3401,39 +3424,39 @@
         <v>6.2</v>
       </c>
       <c r="B91" s="2">
+        <v>4</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A92" s="35">
+        <v>6.2</v>
+      </c>
+      <c r="B92" s="2">
         <v>5</v>
       </c>
-      <c r="C91" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="D91" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="E91" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="F91" s="7" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A92" s="36">
-        <v>7</v>
-      </c>
-      <c r="B92" s="2">
-        <v>1</v>
-      </c>
       <c r="C92" s="18" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>233</v>
+        <v>277</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3441,19 +3464,19 @@
         <v>7</v>
       </c>
       <c r="B93" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>83</v>
+        <v>226</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3464,54 +3487,54 @@
         <v>2</v>
       </c>
       <c r="C94" s="18" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="F94" s="39"/>
-    </row>
-    <row r="95" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="37">
-        <v>8</v>
+        <v>224</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A95" s="36">
+        <v>7</v>
       </c>
       <c r="B95" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A96" s="37">
-        <v>8</v>
-      </c>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A96" s="36"/>
       <c r="B96" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C96" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="E96" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="D96" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>232</v>
-      </c>
       <c r="F96" s="7" t="s">
-        <v>235</v>
+        <v>296</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3519,19 +3542,19 @@
         <v>8</v>
       </c>
       <c r="B97" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C97" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="E97" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="D97" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>232</v>
-      </c>
       <c r="F97" s="7" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3539,23 +3562,40 @@
         <v>8</v>
       </c>
       <c r="B98" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>238</v>
+        <v>297</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F99" s="7"/>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A99" s="37">
+        <v>8</v>
+      </c>
+      <c r="B99" s="2">
+        <v>3</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F100" s="7"/>
@@ -4094,8 +4134,11 @@
     <row r="278" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F278" s="7"/>
     </row>
+    <row r="279" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F279" s="7"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F98"/>
+  <autoFilter ref="A1:F99"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
almost finish fix all logic - missing updating cart after buy
</commit_message>
<xml_diff>
--- a/doc/ver1_fixes/AcceptanceTests - New.xlsx
+++ b/doc/ver1_fixes/AcceptanceTests - New.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$101</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="307">
   <si>
     <t>use case</t>
   </si>
@@ -320,15 +320,6 @@
     <t>{$gitRepo}\dev\main\Service\ServiceFacade.py #buyManyItems</t>
   </si>
   <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems1()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems2()</t>
-  </si>
-  <si>
-    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems3()</t>
-  </si>
-  <si>
     <t>המערכת מודיעה כי אין את הפריטים הרצוים במלאי</t>
   </si>
   <si>
@@ -897,9 +888,6 @@
   </si>
   <si>
     <t>המשתמש האורח רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום תקינים אך פרטי אספקה לא תקינים</t>
-  </si>
-  <si>
-    <t>המערכת הציגה סכום לתשלום והמערכת מודיעה כי פרטי האספקה שגויים והרכישה לא התבצעה</t>
   </si>
   <si>
     <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem8()</t>
@@ -932,6 +920,42 @@
   </si>
   <si>
     <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buySingleItem10()</t>
+  </si>
+  <si>
+    <t>המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות, מזין פרטי אספקה לא תקינים</t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי פרטי האספקה שגויים והרכישה לא התבצעה</t>
+  </si>
+  <si>
+    <t>המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות בקנייה מחנויות שונות</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems2_only_buy_test</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems3_only_buy_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems4_only_buy_test </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems1_only_buy_test  {$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems1_only_supply_test  {$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems1_only_pay_test </t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems5</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems7</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems8</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems9</t>
+  </si>
+  <si>
+    <t>{$gitRepo}\dev\AcceptanceTests\test_acc.py #test_buyManyItems6</t>
   </si>
 </sst>
 </file>
@@ -955,7 +979,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1112,12 +1136,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1168,7 +1186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1277,9 +1295,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1610,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F279"/>
+  <dimension ref="A1:F281"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1704,7 +1719,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1724,7 +1739,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1744,7 +1759,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
@@ -1884,7 +1899,7 @@
         <v>29</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -1915,10 +1930,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>47</v>
@@ -2024,7 +2039,7 @@
         <v>47</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2044,7 +2059,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2064,7 +2079,7 @@
         <v>47</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -2144,7 +2159,7 @@
         <v>74</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2164,7 +2179,7 @@
         <v>74</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2184,7 +2199,7 @@
         <v>74</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
@@ -2204,7 +2219,7 @@
         <v>81</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2235,16 +2250,16 @@
         <v>3</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>81</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2255,16 +2270,16 @@
         <v>4</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>81</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2284,7 +2299,7 @@
         <v>81</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2304,7 +2319,7 @@
         <v>81</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2324,7 +2339,7 @@
         <v>81</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2344,10 +2359,10 @@
         <v>81</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
         <v>91</v>
       </c>
@@ -2363,11 +2378,11 @@
       <c r="E37" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="F37" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
         <v>91</v>
       </c>
@@ -2375,16 +2390,16 @@
         <v>2</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>93</v>
+        <v>297</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>96</v>
+      <c r="F38" s="6" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -2395,63 +2410,67 @@
         <v>3</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F39" s="38"/>
-    </row>
-    <row r="40" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="F39" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
         <v>91</v>
       </c>
       <c r="B40" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="F40" s="6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>101</v>
+        <v>295</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>87</v>
+        <v>296</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="38"/>
-    </row>
-    <row r="42" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="F41" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
         <v>91</v>
       </c>
       <c r="B42" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>80</v>
@@ -2459,64 +2478,68 @@
       <c r="E42" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F42" s="38"/>
+      <c r="F42" s="6" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A43" s="23" t="s">
         <v>91</v>
       </c>
       <c r="B43" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F43" s="38"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="24">
-        <v>3.1</v>
+      <c r="F43" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="B44" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="25">
-        <v>3.1</v>
+        <v>94</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="B45" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>110</v>
+        <v>94</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2524,59 +2547,59 @@
         <v>3.1</v>
       </c>
       <c r="B46" s="2">
+        <v>1</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="25">
+        <v>3.1</v>
+      </c>
+      <c r="B47" s="2">
+        <v>2</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="24">
+        <v>3.1</v>
+      </c>
+      <c r="B48" s="2">
         <v>3</v>
       </c>
-      <c r="C46" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D46" s="18" t="s">
+      <c r="C48" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="26">
-        <v>3.2</v>
-      </c>
-      <c r="B47" s="2">
-        <v>1</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="26">
-        <v>3.2</v>
-      </c>
-      <c r="B48" s="2">
-        <v>2</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>115</v>
-      </c>
       <c r="F48" s="7" t="s">
-        <v>117</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2584,19 +2607,19 @@
         <v>3.2</v>
       </c>
       <c r="B49" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2604,19 +2627,19 @@
         <v>3.2</v>
       </c>
       <c r="B50" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>259</v>
+        <v>116</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>253</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2624,359 +2647,359 @@
         <v>3.2</v>
       </c>
       <c r="B51" s="2">
+        <v>3</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A52" s="26">
+        <v>3.2</v>
+      </c>
+      <c r="B52" s="2">
+        <v>4</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A53" s="26">
+        <v>3.2</v>
+      </c>
+      <c r="B53" s="2">
         <v>5</v>
       </c>
-      <c r="C51" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="B52" s="2">
-        <v>1</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="B53" s="2">
-        <v>2</v>
-      </c>
       <c r="C53" s="18" t="s">
-        <v>122</v>
+        <v>254</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>128</v>
+        <v>255</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>137</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A54" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B54" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="E54" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F54" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A55" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B55" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>231</v>
+        <v>119</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>232</v>
+        <v>125</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>255</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A56" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" s="2">
+        <v>3</v>
+      </c>
+      <c r="C56" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="B56" s="2">
-        <v>5</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>264</v>
-      </c>
       <c r="D56" s="18" t="s">
-        <v>233</v>
+        <v>143</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A57" s="27" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B57" s="2">
+        <v>4</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A58" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" s="2">
+        <v>5</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="2">
         <v>6</v>
       </c>
-      <c r="C57" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A58" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="B58" s="2">
-        <v>1</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A59" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="B59" s="2">
-        <v>2</v>
-      </c>
       <c r="C59" s="18" t="s">
-        <v>124</v>
+        <v>262</v>
       </c>
       <c r="D59" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="E59" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E59" s="10" t="s">
-        <v>134</v>
-      </c>
       <c r="F59" s="7" t="s">
-        <v>139</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A60" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B60" s="2">
+        <v>1</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A61" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61" s="2">
+        <v>2</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A62" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="2">
         <v>3</v>
       </c>
-      <c r="C60" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A61" s="29" t="s">
+      <c r="C62" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B61" s="2">
-        <v>1</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="D61" s="18" t="s">
+      <c r="D62" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E62" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E61" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A62" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="B62" s="2">
-        <v>2</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>135</v>
-      </c>
       <c r="F62" s="7" t="s">
-        <v>141</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A63" s="29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B63" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>260</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A64" s="29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B64" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>234</v>
+        <v>123</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>237</v>
+        <v>129</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>261</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A65" s="29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B65" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>235</v>
+        <v>146</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A66" s="29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B66" s="2">
+        <v>4</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A67" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B67" s="2">
+        <v>5</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A68" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="2">
         <v>6</v>
       </c>
-      <c r="C66" s="18" t="s">
+      <c r="C68" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="D68" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="D66" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A67" s="30">
-        <v>4.3</v>
-      </c>
-      <c r="B67" s="2">
-        <v>1</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E67" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="30">
-        <v>4.3</v>
-      </c>
-      <c r="B68" s="2">
-        <v>2</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>155</v>
-      </c>
       <c r="E68" s="10" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>160</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -2984,19 +3007,19 @@
         <v>4.3</v>
       </c>
       <c r="B69" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D69" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F69" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3004,19 +3027,19 @@
         <v>4.3</v>
       </c>
       <c r="B70" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D70" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F70" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3024,299 +3047,299 @@
         <v>4.3</v>
       </c>
       <c r="B71" s="2">
+        <v>3</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="30">
+        <v>4.3</v>
+      </c>
+      <c r="B72" s="2">
+        <v>4</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A73" s="30">
+        <v>4.3</v>
+      </c>
+      <c r="B73" s="2">
         <v>5</v>
       </c>
-      <c r="C71" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="31">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B72" s="2">
-        <v>1</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="31">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B73" s="2">
-        <v>2</v>
-      </c>
       <c r="C73" s="18" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A74" s="31">
         <v>4.4000000000000004</v>
       </c>
       <c r="B74" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>170</v>
+        <v>270</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A75" s="31">
         <v>4.4000000000000004</v>
       </c>
       <c r="B75" s="2">
+        <v>2</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A76" s="31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B76" s="2">
+        <v>3</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A77" s="31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B77" s="2">
         <v>4</v>
       </c>
-      <c r="C75" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="D75" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="32">
-        <v>4.5</v>
-      </c>
-      <c r="B76" s="2">
-        <v>1</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="D76" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E76" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A77" s="32">
-        <v>4.5</v>
-      </c>
-      <c r="B77" s="2">
-        <v>2</v>
-      </c>
       <c r="C77" s="18" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A78" s="32">
         <v>4.5</v>
       </c>
       <c r="B78" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A79" s="32">
         <v>4.5</v>
       </c>
       <c r="B79" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A80" s="32">
         <v>4.5</v>
       </c>
       <c r="B80" s="2">
+        <v>3</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A81" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="B81" s="2">
+        <v>4</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="B82" s="2">
         <v>5</v>
       </c>
-      <c r="C80" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="D80" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A81" s="33">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="B81" s="2">
-        <v>1</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="D81" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A82" s="33">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="B82" s="2">
-        <v>2</v>
-      </c>
       <c r="C82" s="18" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A83" s="33">
         <v>4.5999999999999996</v>
       </c>
       <c r="B83" s="2">
+        <v>1</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="33">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B84" s="2">
+        <v>2</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A85" s="33">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B85" s="2">
         <v>3</v>
       </c>
-      <c r="C83" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="D83" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="E83" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A84" s="34">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B84" s="2">
-        <v>1</v>
-      </c>
-      <c r="C84" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="D84" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="E84" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="34">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B85" s="2">
-        <v>2</v>
-      </c>
       <c r="C85" s="18" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>134</v>
+        <v>190</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>139</v>
+        <v>272</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3324,79 +3347,79 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B86" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86" s="18" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A87" s="34">
         <v>5.0999999999999996</v>
       </c>
       <c r="B87" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D87" s="18" t="s">
         <v>201</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A88" s="35">
-        <v>6.2</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A88" s="34">
+        <v>5.0999999999999996</v>
       </c>
       <c r="B88" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>208</v>
+        <v>131</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A89" s="35">
-        <v>6.2</v>
+      <c r="A89" s="34">
+        <v>5.0999999999999996</v>
       </c>
       <c r="B89" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C89" s="18" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>208</v>
+        <v>131</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>210</v>
+        <v>275</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3404,19 +3427,19 @@
         <v>6.2</v>
       </c>
       <c r="B90" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3424,19 +3447,19 @@
         <v>6.2</v>
       </c>
       <c r="B91" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C91" s="18" t="s">
-        <v>279</v>
+        <v>203</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>276</v>
+        <v>207</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3444,59 +3467,59 @@
         <v>6.2</v>
       </c>
       <c r="B92" s="2">
+        <v>3</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A93" s="35">
+        <v>6.2</v>
+      </c>
+      <c r="B93" s="2">
+        <v>4</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A94" s="35">
+        <v>6.2</v>
+      </c>
+      <c r="B94" s="2">
         <v>5</v>
       </c>
-      <c r="C92" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="D92" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="E92" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A93" s="36">
-        <v>7</v>
-      </c>
-      <c r="B93" s="2">
-        <v>1</v>
-      </c>
-      <c r="C93" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="D93" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="E93" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="F93" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A94" s="36">
-        <v>7</v>
-      </c>
-      <c r="B94" s="2">
-        <v>2</v>
-      </c>
       <c r="C94" s="18" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
@@ -3504,77 +3527,77 @@
         <v>7</v>
       </c>
       <c r="B95" s="2">
+        <v>1</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A96" s="36">
+        <v>7</v>
+      </c>
+      <c r="B96" s="2">
+        <v>2</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A97" s="36">
+        <v>7</v>
+      </c>
+      <c r="B97" s="2">
         <v>3</v>
       </c>
-      <c r="C95" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="D95" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A96" s="36"/>
-      <c r="B96" s="2">
+      <c r="C97" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A98" s="36"/>
+      <c r="B98" s="2">
         <v>4</v>
       </c>
-      <c r="C96" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="D96" s="18" t="s">
+      <c r="C98" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F98" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A97" s="37">
-        <v>8</v>
-      </c>
-      <c r="B97" s="2">
-        <v>1</v>
-      </c>
-      <c r="C97" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="D97" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="F97" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A98" s="37">
-        <v>8</v>
-      </c>
-      <c r="B98" s="2">
-        <v>2</v>
-      </c>
-      <c r="C98" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="D98" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="E98" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -3582,26 +3605,60 @@
         <v>8</v>
       </c>
       <c r="B99" s="2">
+        <v>1</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A100" s="37">
+        <v>8</v>
+      </c>
+      <c r="B100" s="2">
+        <v>2</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="D100" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A101" s="37">
+        <v>8</v>
+      </c>
+      <c r="B101" s="2">
         <v>3</v>
       </c>
-      <c r="C99" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="D99" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="E99" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="F99" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F100" s="7"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F101" s="7"/>
+      <c r="C101" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F102" s="7"/>
@@ -4137,8 +4194,14 @@
     <row r="279" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F279" s="7"/>
     </row>
+    <row r="280" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F280" s="7"/>
+    </row>
+    <row r="281" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F281" s="7"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F99"/>
+  <autoFilter ref="A1:F101"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>